<commit_message>
changes on excel procedures
</commit_message>
<xml_diff>
--- a/entregaFinal/src/loginData.xlsx
+++ b/entregaFinal/src/loginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\git\entregafinal\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\selenium\entregaFinal\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0A3852-301A-46B1-9017-C75779F2C74E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEC5983-F3D3-4715-9E9A-2802F24AB70D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="8295" xr2:uid="{FA9E2868-C39F-42AC-8CF2-8679C1D4CDCB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" xr2:uid="{FA9E2868-C39F-42AC-8CF2-8679C1D4CDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -399,12 +400,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,11 +413,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1234</v>
       </c>
     </row>
@@ -425,5 +426,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D34349A9-F123-4298-BBA5-1B42E1D5FF05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>